<commit_message>
Postpaid take-out Flow WO TIP
</commit_message>
<xml_diff>
--- a/src/test/resources/Sheet/Configsheet - Copy.xlsx
+++ b/src/test/resources/Sheet/Configsheet - Copy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jones\eclipse-workspace\Automation-QAPlateron\src\test\resources\Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBE485D3-618C-4CF2-AD92-AFFF2253B29E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C3E692-80BE-4B07-8614-3348543E6A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill Configuration" sheetId="3" r:id="rId1"/>
@@ -21,29 +21,26 @@
     <sheet name="Table List" sheetId="6" r:id="rId6"/>
     <sheet name="Discount" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="164">
-  <si>
-    <t>Employee Name</t>
-  </si>
-  <si>
-    <t>EmpRole</t>
-  </si>
-  <si>
-    <t>PIN</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="184">
   <si>
     <t>PhoneNo</t>
   </si>
@@ -534,6 +531,78 @@
   </si>
   <si>
     <t>Auto 7</t>
+  </si>
+  <si>
+    <t>+1 (777) 777 - 7723</t>
+  </si>
+  <si>
+    <t>+1 (904) 244 - 7113</t>
+  </si>
+  <si>
+    <t>+1 (599) 810 - 5189</t>
+  </si>
+  <si>
+    <t>+1 (874) 921 - 1379</t>
+  </si>
+  <si>
+    <t>+1 (194) 044 - 5345</t>
+  </si>
+  <si>
+    <t>Employee Name</t>
+  </si>
+  <si>
+    <t>EmpRole</t>
+  </si>
+  <si>
+    <t>PIN</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>Q A</t>
+  </si>
+  <si>
+    <t>Owner</t>
+  </si>
+  <si>
+    <t>4567</t>
+  </si>
+  <si>
+    <t>qa@gmail.com</t>
+  </si>
+  <si>
+    <t>AutTest34</t>
+  </si>
+  <si>
+    <t>Manager</t>
+  </si>
+  <si>
+    <t>7115</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>5997</t>
+  </si>
+  <si>
+    <t>NZxFqkOy0k</t>
+  </si>
+  <si>
+    <t>Busser</t>
+  </si>
+  <si>
+    <t>7028</t>
+  </si>
+  <si>
+    <t>PwyfyzLP6F</t>
+  </si>
+  <si>
+    <t>Waiter</t>
+  </si>
+  <si>
+    <t>2557</t>
   </si>
 </sst>
 </file>
@@ -659,7 +728,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -692,6 +761,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -975,7 +1045,7 @@
   <dimension ref="A1:B17"/>
   <sheetViews>
     <sheetView zoomScale="70" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -986,15 +1056,15 @@
   <sheetData>
     <row r="1" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A2" s="3" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B2" s="4">
         <v>66.66</v>
@@ -1002,23 +1072,23 @@
     </row>
     <row r="3" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A3" s="3" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A4" s="3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A5" s="3" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="B5" s="4">
         <v>33.33</v>
@@ -1026,15 +1096,15 @@
     </row>
     <row r="6" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A6" s="3" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A7" s="3" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B7" s="4">
         <v>33.33</v>
@@ -1042,31 +1112,31 @@
     </row>
     <row r="8" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A8" s="3" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A9" s="3" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A10" s="3" t="s">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A11" s="3" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="B11" s="4">
         <v>75.989999999999995</v>
@@ -1074,7 +1144,7 @@
     </row>
     <row r="12" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A12" s="3" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="B12" s="4">
         <v>12</v>
@@ -1082,15 +1152,15 @@
     </row>
     <row r="13" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A13" s="3" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="B13" s="4">
-        <v>99</v>
+        <v>5</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A14" s="3" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B14" s="4">
         <v>51</v>
@@ -1098,26 +1168,26 @@
     </row>
     <row r="15" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A15" s="3" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A16" s="3" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A17" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
     </row>
   </sheetData>
@@ -1128,10 +1198,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:E23"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1145,19 +1215,104 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C1" t="s">
+        <v>167</v>
+      </c>
+      <c r="D1" t="s">
+        <v>168</v>
+      </c>
+      <c r="E1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>169</v>
+      </c>
+      <c r="B2" t="s">
+        <v>170</v>
+      </c>
+      <c r="C2" t="s">
+        <v>171</v>
+      </c>
+      <c r="D2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E2" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>173</v>
+      </c>
+      <c r="B3" t="s">
+        <v>174</v>
+      </c>
+      <c r="C3" t="s">
+        <v>175</v>
+      </c>
+      <c r="D3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>173</v>
+      </c>
+      <c r="B4" t="s">
+        <v>174</v>
+      </c>
+      <c r="C4" t="s">
+        <v>177</v>
+      </c>
+      <c r="D4" t="s">
+        <v>176</v>
+      </c>
+      <c r="E4" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>178</v>
+      </c>
+      <c r="B5" t="s">
+        <v>179</v>
+      </c>
+      <c r="C5" t="s">
+        <v>180</v>
+      </c>
+      <c r="D5" t="s">
+        <v>176</v>
+      </c>
+      <c r="E5" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>181</v>
+      </c>
+      <c r="B6" t="s">
+        <v>182</v>
+      </c>
+      <c r="C6" t="s">
+        <v>183</v>
+      </c>
+      <c r="D6" t="s">
+        <v>176</v>
+      </c>
+      <c r="E6" t="s">
+        <v>164</v>
       </c>
     </row>
   </sheetData>
@@ -1183,338 +1338,338 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B2" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C2" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="D2" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="C3" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="D3" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B4" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="C4" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D4" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B5" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C5" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="D5" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B6" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="C6" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="D6" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B7" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C7" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="D7" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B8" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="C8" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="D8" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B9" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="C9" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D9" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B10" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="C10" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="D10" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="B11" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="C11" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="D11" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B12" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="C12" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="D12" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B13" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="C13" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="D13" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B14" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="C14" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="D14" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B15" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="C15" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="D15" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B16" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C16" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="D16" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B17" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="C17" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="D17" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B18" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="C18" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="D18" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B19" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="C19" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="D19" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B20" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="C20" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="D20" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="B21" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="C21" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="D21" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B22" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="C22" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22" t="s">
         <v>91</v>
-      </c>
-      <c r="D22" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="B23" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="C23" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="D23" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
+        <v>130</v>
+      </c>
+      <c r="B24" t="s">
+        <v>133</v>
+      </c>
+      <c r="C24" t="s">
         <v>134</v>
       </c>
-      <c r="B24" t="s">
-        <v>137</v>
-      </c>
-      <c r="C24" t="s">
-        <v>138</v>
-      </c>
       <c r="D24" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1539,145 +1694,145 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="C2" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B3" t="s">
+        <v>71</v>
+      </c>
+      <c r="C3" t="s">
         <v>72</v>
-      </c>
-      <c r="B3" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="C4" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="B5" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B6" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="C6" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B7" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="C7" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C8" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>76</v>
+      </c>
+      <c r="B9" t="s">
         <v>80</v>
       </c>
-      <c r="B9" t="s">
-        <v>84</v>
-      </c>
       <c r="C9" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="C10" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B11" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C11" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="B12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" t="s">
         <v>85</v>
       </c>
-      <c r="B13" t="s">
-        <v>89</v>
-      </c>
       <c r="C13" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -1709,426 +1864,426 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="F1" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="G1" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="H1" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="E1" s="6" t="s">
+      <c r="I1" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="J1" s="6" t="s">
         <v>37</v>
-      </c>
-      <c r="G1" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="I1" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="J1" s="6" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B2" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D2" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E2" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F2" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H2" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="I2" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B3" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D3" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E3" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G3" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="I3" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J3" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B4" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D4" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E4" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F4" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G4" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="I4" s="8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="J4" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B5" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D5" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F5" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G5" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="I5" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J5" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="B6" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D6" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H6" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="I6" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="J6" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B7" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D7" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F7" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="I7" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J7" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="B8" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G8" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="I8" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="B9" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D9" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G9" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="I9" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J9" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="B10" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G10" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="I10" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="J10" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B11" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G11" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H11" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="I11" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J11" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B12" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G12" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="H12" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="I12" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="J12" s="8" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G13" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="I13" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="J13" s="8" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="B14" s="10" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -2149,112 +2304,112 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="B1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="B2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="C3" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B4" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="C4" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B5" t="s">
         <v>145</v>
       </c>
-      <c r="B5" t="s">
-        <v>149</v>
-      </c>
       <c r="C5" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B6" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="C6" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="B7" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="C7" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="B8" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
       <c r="C8" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="B9" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C9" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="B10" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="C10" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
     </row>
   </sheetData>
@@ -2266,8 +2421,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DA6CF15C-C633-4176-8909-CF9532871AF5}">
   <dimension ref="A1:H8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2283,192 +2438,192 @@
   <sheetData>
     <row r="1" spans="1:8" s="14" customFormat="1" ht="17.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="D1" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="F1" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C1" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="D1" s="11" t="s">
-        <v>61</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>62</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>63</v>
-      </c>
       <c r="G1" s="13" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="H1" s="13" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B2" s="7">
-        <v>23</v>
+        <v>60</v>
+      </c>
+      <c r="B2" s="16">
+        <v>21</v>
       </c>
       <c r="C2" s="7">
         <v>0</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G2" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="H2" s="15" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="B3" s="7">
+        <v>61</v>
+      </c>
+      <c r="B3" s="16">
         <v>66.66</v>
       </c>
       <c r="C3" s="7">
         <v>130</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E3" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G3" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B4" s="7">
+        <v>62</v>
+      </c>
+      <c r="B4" s="16">
         <v>28.88</v>
       </c>
       <c r="C4" s="7">
         <v>51</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E4" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G4" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="B5" s="7">
+        <v>63</v>
+      </c>
+      <c r="B5" s="16">
         <v>40</v>
       </c>
       <c r="C5" s="7">
         <v>110</v>
       </c>
       <c r="D5" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="E5" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G5" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" s="7">
+        <v>64</v>
+      </c>
+      <c r="B6" s="16">
         <v>24</v>
       </c>
       <c r="C6" s="7">
         <v>19</v>
       </c>
       <c r="D6" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E6" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G6" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7" s="7">
+        <v>65</v>
+      </c>
+      <c r="B7" s="16">
         <v>23.33</v>
       </c>
       <c r="C7" s="7">
         <v>70</v>
       </c>
       <c r="D7" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E7" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="G7" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>163</v>
-      </c>
-      <c r="B8" s="7">
+        <v>159</v>
+      </c>
+      <c r="B8" s="16">
         <v>50</v>
       </c>
       <c r="C8" s="7">
         <v>50</v>
       </c>
       <c r="D8" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G8" s="7" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
POS Dine-In Prepaid flow update part-1
</commit_message>
<xml_diff>
--- a/src/test/resources/Sheet/Configsheet - Copy.xlsx
+++ b/src/test/resources/Sheet/Configsheet - Copy.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jones\eclipse-workspace\Automation-QAPlateron\src\test\resources\Sheet\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5C3E692-80BE-4B07-8614-3348543E6A88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{742EF3C3-D761-46F0-B345-6EC6AE35E149}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Bill Configuration" sheetId="3" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="Jobs Configuration" sheetId="1" r:id="rId5"/>
     <sheet name="Table List" sheetId="6" r:id="rId6"/>
     <sheet name="Discount" sheetId="7" r:id="rId7"/>
+    <sheet name="Reports" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="398" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="118">
   <si>
     <t>PhoneNo</t>
   </si>
@@ -257,205 +258,7 @@
     <t>Deleting Template</t>
   </si>
   <si>
-    <t>Test1</t>
-  </si>
-  <si>
-    <t>Item1</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>Item2</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Item3</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>Item4</t>
-  </si>
-  <si>
-    <t>Test2</t>
-  </si>
-  <si>
-    <t>Item5</t>
-  </si>
-  <si>
-    <t>Item6</t>
-  </si>
-  <si>
-    <t>Item7</t>
-  </si>
-  <si>
-    <t>Item8</t>
-  </si>
-  <si>
-    <t>Test3</t>
-  </si>
-  <si>
-    <t>Item9</t>
-  </si>
-  <si>
-    <t>Item10</t>
-  </si>
-  <si>
-    <t>Item11</t>
-  </si>
-  <si>
-    <t>Item12</t>
-  </si>
-  <si>
-    <t>Menu Item1</t>
-  </si>
-  <si>
-    <t>1.99</t>
-  </si>
-  <si>
-    <t>Vegetarian</t>
-  </si>
-  <si>
-    <t>Menu Item2</t>
-  </si>
-  <si>
-    <t>2.99</t>
-  </si>
-  <si>
-    <t>Non-Vegetarian</t>
-  </si>
-  <si>
-    <t>Menu Item3</t>
-  </si>
-  <si>
-    <t>3.99</t>
-  </si>
-  <si>
-    <t>Vegan</t>
-  </si>
-  <si>
-    <t>Menu Item4</t>
-  </si>
-  <si>
-    <t>4.99</t>
-  </si>
-  <si>
-    <t>Menu Item5</t>
-  </si>
-  <si>
-    <t>5</t>
-  </si>
-  <si>
-    <t>Menu Item6</t>
-  </si>
-  <si>
-    <t>6.99</t>
-  </si>
-  <si>
-    <t>Menu Item7</t>
-  </si>
-  <si>
-    <t>75</t>
-  </si>
-  <si>
-    <t>Menu Item8</t>
-  </si>
-  <si>
-    <t>8.99</t>
-  </si>
-  <si>
-    <t>Menu Item9</t>
-  </si>
-  <si>
-    <t>9.99</t>
-  </si>
-  <si>
-    <t>Menu Item10</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>Menu Item11</t>
-  </si>
-  <si>
-    <t>100</t>
-  </si>
-  <si>
-    <t>Menu Item12</t>
-  </si>
-  <si>
-    <t>Menu Item13</t>
-  </si>
-  <si>
-    <t>20</t>
-  </si>
-  <si>
-    <t>Menu Item14</t>
-  </si>
-  <si>
-    <t>33.33</t>
-  </si>
-  <si>
-    <t>Menu Item15</t>
-  </si>
-  <si>
-    <t>66.66</t>
-  </si>
-  <si>
-    <t>Menu Item16</t>
-  </si>
-  <si>
-    <t>22.22</t>
-  </si>
-  <si>
-    <t>Menu Item17</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t>Menu Item18</t>
-  </si>
-  <si>
-    <t>0.99</t>
-  </si>
-  <si>
-    <t>Menu Item19</t>
-  </si>
-  <si>
     <t>12</t>
-  </si>
-  <si>
-    <t>Menu Item20</t>
-  </si>
-  <si>
-    <t>13.99</t>
-  </si>
-  <si>
-    <t>1Vf5l03Bu1</t>
-  </si>
-  <si>
-    <t>sUH1pn9ewL</t>
-  </si>
-  <si>
-    <t>W8nkKnuIUD</t>
-  </si>
-  <si>
-    <t>MenuModifier1</t>
-  </si>
-  <si>
-    <t>MenuModifier2</t>
-  </si>
-  <si>
-    <t>MenuModifier3</t>
-  </si>
-  <si>
-    <t>7.99</t>
   </si>
   <si>
     <t>Area Name</t>
@@ -651,7 +454,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -673,6 +476,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -728,7 +537,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -762,6 +571,7 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1200,7 +1010,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E6"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
@@ -1215,16 +1025,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>165</v>
+        <v>99</v>
       </c>
       <c r="B1" t="s">
-        <v>166</v>
+        <v>100</v>
       </c>
       <c r="C1" t="s">
-        <v>167</v>
+        <v>101</v>
       </c>
       <c r="D1" t="s">
-        <v>168</v>
+        <v>102</v>
       </c>
       <c r="E1" t="s">
         <v>0</v>
@@ -1232,87 +1042,87 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>169</v>
+        <v>103</v>
       </c>
       <c r="B2" t="s">
-        <v>170</v>
+        <v>104</v>
       </c>
       <c r="C2" t="s">
-        <v>171</v>
+        <v>105</v>
       </c>
       <c r="D2" t="s">
-        <v>172</v>
+        <v>106</v>
       </c>
       <c r="E2" t="s">
-        <v>160</v>
+        <v>94</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>173</v>
+        <v>107</v>
       </c>
       <c r="B3" t="s">
-        <v>174</v>
+        <v>108</v>
       </c>
       <c r="C3" t="s">
-        <v>175</v>
+        <v>109</v>
       </c>
       <c r="D3" t="s">
-        <v>176</v>
+        <v>110</v>
       </c>
       <c r="E3" t="s">
-        <v>161</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>173</v>
+        <v>107</v>
       </c>
       <c r="B4" t="s">
-        <v>174</v>
+        <v>108</v>
       </c>
       <c r="C4" t="s">
-        <v>177</v>
+        <v>111</v>
       </c>
       <c r="D4" t="s">
-        <v>176</v>
+        <v>110</v>
       </c>
       <c r="E4" t="s">
-        <v>162</v>
+        <v>96</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>178</v>
+        <v>112</v>
       </c>
       <c r="B5" t="s">
-        <v>179</v>
+        <v>113</v>
       </c>
       <c r="C5" t="s">
-        <v>180</v>
+        <v>114</v>
       </c>
       <c r="D5" t="s">
-        <v>176</v>
+        <v>110</v>
       </c>
       <c r="E5" t="s">
-        <v>163</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>181</v>
+        <v>115</v>
       </c>
       <c r="B6" t="s">
-        <v>182</v>
+        <v>116</v>
       </c>
       <c r="C6" t="s">
-        <v>183</v>
+        <v>117</v>
       </c>
       <c r="D6" t="s">
-        <v>176</v>
+        <v>110</v>
       </c>
       <c r="E6" t="s">
-        <v>164</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>
@@ -1337,341 +1147,117 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="17" t="s">
         <v>22</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="17" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>128</v>
-      </c>
-      <c r="B2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C2" t="s">
-        <v>87</v>
-      </c>
-      <c r="D2" t="s">
-        <v>88</v>
-      </c>
+      <c r="A2"/>
+      <c r="B2"/>
+      <c r="C2"/>
+      <c r="D2"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D3" t="s">
-        <v>91</v>
-      </c>
+      <c r="A3"/>
+      <c r="B3"/>
+      <c r="C3"/>
+      <c r="D3"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>128</v>
-      </c>
-      <c r="B4" t="s">
-        <v>92</v>
-      </c>
-      <c r="C4" t="s">
-        <v>93</v>
-      </c>
-      <c r="D4" t="s">
-        <v>94</v>
-      </c>
+      <c r="A4"/>
+      <c r="B4"/>
+      <c r="C4"/>
+      <c r="D4"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>128</v>
-      </c>
-      <c r="B5" t="s">
-        <v>95</v>
-      </c>
-      <c r="C5" t="s">
-        <v>96</v>
-      </c>
-      <c r="D5" t="s">
-        <v>88</v>
-      </c>
+      <c r="A5"/>
+      <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>128</v>
-      </c>
-      <c r="B6" t="s">
-        <v>97</v>
-      </c>
-      <c r="C6" t="s">
-        <v>98</v>
-      </c>
-      <c r="D6" t="s">
-        <v>91</v>
-      </c>
+      <c r="A6"/>
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="D6"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>128</v>
-      </c>
-      <c r="B7" t="s">
-        <v>99</v>
-      </c>
-      <c r="C7" t="s">
-        <v>100</v>
-      </c>
-      <c r="D7" t="s">
-        <v>94</v>
-      </c>
+      <c r="A7"/>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>128</v>
-      </c>
-      <c r="B8" t="s">
-        <v>101</v>
-      </c>
-      <c r="C8" t="s">
-        <v>102</v>
-      </c>
-      <c r="D8" t="s">
-        <v>88</v>
-      </c>
+      <c r="A8"/>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>128</v>
-      </c>
-      <c r="B9" t="s">
-        <v>103</v>
-      </c>
-      <c r="C9" t="s">
-        <v>104</v>
-      </c>
-      <c r="D9" t="s">
-        <v>91</v>
-      </c>
+      <c r="A9"/>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>128</v>
-      </c>
-      <c r="B10" t="s">
-        <v>105</v>
-      </c>
-      <c r="C10" t="s">
-        <v>106</v>
-      </c>
-      <c r="D10" t="s">
-        <v>94</v>
-      </c>
+      <c r="A10"/>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>128</v>
-      </c>
-      <c r="B11" t="s">
-        <v>107</v>
-      </c>
-      <c r="C11" t="s">
-        <v>108</v>
-      </c>
-      <c r="D11" t="s">
-        <v>88</v>
-      </c>
+      <c r="A11"/>
+      <c r="B11"/>
+      <c r="C11"/>
+      <c r="D11"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>129</v>
-      </c>
-      <c r="B12" t="s">
-        <v>109</v>
-      </c>
-      <c r="C12" t="s">
-        <v>110</v>
-      </c>
-      <c r="D12" t="s">
-        <v>91</v>
-      </c>
+      <c r="A12"/>
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>129</v>
-      </c>
-      <c r="B13" t="s">
-        <v>111</v>
-      </c>
-      <c r="C13" t="s">
-        <v>70</v>
-      </c>
-      <c r="D13" t="s">
-        <v>94</v>
-      </c>
+      <c r="A13"/>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>129</v>
-      </c>
-      <c r="B14" t="s">
-        <v>112</v>
-      </c>
-      <c r="C14" t="s">
-        <v>113</v>
-      </c>
-      <c r="D14" t="s">
-        <v>94</v>
-      </c>
+      <c r="A14"/>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>129</v>
-      </c>
-      <c r="B15" t="s">
-        <v>114</v>
-      </c>
-      <c r="C15" t="s">
-        <v>115</v>
-      </c>
-      <c r="D15" t="s">
-        <v>94</v>
-      </c>
+      <c r="A15"/>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>129</v>
-      </c>
-      <c r="B16" t="s">
-        <v>116</v>
-      </c>
-      <c r="C16" t="s">
-        <v>117</v>
-      </c>
-      <c r="D16" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>129</v>
-      </c>
-      <c r="B17" t="s">
-        <v>118</v>
-      </c>
-      <c r="C17" t="s">
-        <v>119</v>
-      </c>
-      <c r="D17" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>129</v>
-      </c>
-      <c r="B18" t="s">
-        <v>120</v>
-      </c>
-      <c r="C18" t="s">
-        <v>121</v>
-      </c>
-      <c r="D18" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>129</v>
-      </c>
-      <c r="B19" t="s">
-        <v>122</v>
-      </c>
-      <c r="C19" t="s">
-        <v>123</v>
-      </c>
-      <c r="D19" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>129</v>
-      </c>
-      <c r="B20" t="s">
-        <v>124</v>
-      </c>
-      <c r="C20" t="s">
-        <v>125</v>
-      </c>
-      <c r="D20" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>129</v>
-      </c>
-      <c r="B21" t="s">
-        <v>126</v>
-      </c>
-      <c r="C21" t="s">
-        <v>127</v>
-      </c>
-      <c r="D21" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>130</v>
-      </c>
-      <c r="B22" t="s">
-        <v>131</v>
-      </c>
-      <c r="C22" t="s">
-        <v>87</v>
-      </c>
-      <c r="D22" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>130</v>
-      </c>
-      <c r="B23" t="s">
-        <v>132</v>
-      </c>
-      <c r="C23" t="s">
-        <v>93</v>
-      </c>
-      <c r="D23" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>130</v>
-      </c>
-      <c r="B24" t="s">
-        <v>133</v>
-      </c>
-      <c r="C24" t="s">
-        <v>134</v>
-      </c>
-      <c r="D24" t="s">
-        <v>94</v>
-      </c>
-    </row>
+      <c r="A16"/>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+    </row>
+    <row r="17" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="18" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="20" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="21" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="22" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="23" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="24" customFormat="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1679,10 +1265,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1701,138 +1287,6 @@
       </c>
       <c r="C1" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" t="s">
-        <v>69</v>
-      </c>
-      <c r="C2" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B3" t="s">
-        <v>71</v>
-      </c>
-      <c r="C3" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B4" t="s">
-        <v>73</v>
-      </c>
-      <c r="C4" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>68</v>
-      </c>
-      <c r="B5" t="s">
-        <v>75</v>
-      </c>
-      <c r="C5" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>76</v>
-      </c>
-      <c r="B6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>76</v>
-      </c>
-      <c r="B7" t="s">
-        <v>78</v>
-      </c>
-      <c r="C7" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>76</v>
-      </c>
-      <c r="B8" t="s">
-        <v>79</v>
-      </c>
-      <c r="C8" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>76</v>
-      </c>
-      <c r="B9" t="s">
-        <v>80</v>
-      </c>
-      <c r="C9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>81</v>
-      </c>
-      <c r="B10" t="s">
-        <v>82</v>
-      </c>
-      <c r="C10" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>81</v>
-      </c>
-      <c r="B11" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>81</v>
-      </c>
-      <c r="B12" t="s">
-        <v>84</v>
-      </c>
-      <c r="C12" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>81</v>
-      </c>
-      <c r="B13" t="s">
-        <v>85</v>
-      </c>
-      <c r="C13" t="s">
-        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -2304,112 +1758,112 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>135</v>
+        <v>69</v>
       </c>
       <c r="B1" t="s">
-        <v>136</v>
+        <v>70</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>138</v>
+        <v>72</v>
       </c>
       <c r="B2" t="s">
-        <v>139</v>
+        <v>73</v>
       </c>
       <c r="C2" t="s">
-        <v>140</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>141</v>
+        <v>75</v>
       </c>
       <c r="B3" t="s">
-        <v>142</v>
+        <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>140</v>
+        <v>74</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>141</v>
+        <v>75</v>
       </c>
       <c r="B4" t="s">
-        <v>143</v>
+        <v>77</v>
       </c>
       <c r="C4" t="s">
-        <v>144</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>141</v>
+        <v>75</v>
       </c>
       <c r="B5" t="s">
-        <v>145</v>
+        <v>79</v>
       </c>
       <c r="C5" t="s">
-        <v>146</v>
+        <v>80</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>141</v>
+        <v>75</v>
       </c>
       <c r="B6" t="s">
-        <v>147</v>
+        <v>81</v>
       </c>
       <c r="C6" t="s">
-        <v>148</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>141</v>
+        <v>75</v>
       </c>
       <c r="B7" t="s">
-        <v>149</v>
+        <v>83</v>
       </c>
       <c r="C7" t="s">
-        <v>150</v>
+        <v>84</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>151</v>
+        <v>85</v>
       </c>
       <c r="B8" t="s">
-        <v>152</v>
+        <v>86</v>
       </c>
       <c r="C8" t="s">
-        <v>125</v>
+        <v>68</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>153</v>
+        <v>87</v>
       </c>
       <c r="B9" t="s">
-        <v>154</v>
+        <v>88</v>
       </c>
       <c r="C9" t="s">
-        <v>155</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>156</v>
+        <v>90</v>
       </c>
       <c r="B10" t="s">
-        <v>157</v>
+        <v>91</v>
       </c>
       <c r="C10" t="s">
-        <v>158</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2605,7 +2059,7 @@
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>159</v>
+        <v>93</v>
       </c>
       <c r="B8" s="16">
         <v>50</v>
@@ -2630,4 +2084,18 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB5E0FD6-1845-4CC8-BFCE-C6EAE9737E71}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>